<commit_message>
add function to print the order of init val p0 for fitting
</commit_message>
<xml_diff>
--- a/examples/sample_data/ref6/ref6.xlsx
+++ b/examples/sample_data/ref6/ref6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mt_oh\DataScience\rxnfit\examples\sample_data\ref6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CBEFC0-F6CD-456E-9604-8B2F2336E438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFE4888-751A-42EB-B28B-69BAAD101B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{0E1539FD-C77D-41D1-B5B0-DBFB2F7E988B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>min</t>
     <phoneticPr fontId="1"/>
@@ -110,19 +110,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>diol</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>diacid</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>polyest</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>H2O</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -156,11 +144,52 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>Mn</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>H2O_wt</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Tot_wt</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AdA_mol</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DEG_mol</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DEG</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AdA</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mnは10^-6倍した数値</t>
+    <rPh sb="8" eb="9">
+      <t>バイ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>スウチ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -212,7 +241,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -220,6 +249,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -557,13 +589,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A48E1FF-6AAD-4C3E-B380-DA82EB820F5D}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -574,22 +606,34 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="O1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -600,18 +644,40 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <f>$J$9*(1-B2)</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>$P$9*(1-B2)</f>
         <v>3.9641639578212957</v>
       </c>
-      <c r="E2">
-        <f>$K$9*(1-B2)</f>
+      <c r="F2">
+        <f>$Q$9*(1-B2)</f>
         <v>3.9641639578212957</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2">
+        <f>$P$9*B2*18.02</f>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>1000-H2</f>
+        <v>1000</v>
+      </c>
+      <c r="J2">
+        <f>E2/I2</f>
+        <v>3.9641639578212959E-3</v>
+      </c>
+      <c r="K2">
+        <f>F2/I2</f>
+        <v>3.9641639578212959E-3</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="O2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>6</v>
       </c>
@@ -622,18 +688,42 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="D3">
-        <f>$J$9*(1-B3)</f>
+        <f>(C3*$R$8+18.02)*0.000001</f>
+        <v>2.688352E-4</v>
+      </c>
+      <c r="E3">
+        <f>$P$9*(1-B3)</f>
         <v>3.4175057480377391</v>
       </c>
-      <c r="E3">
-        <f>$K$9*(1-B3)</f>
+      <c r="F3">
+        <f>$Q$9*(1-B3)</f>
         <v>3.4175057480377391</v>
       </c>
-      <c r="I3" t="s">
+      <c r="H3">
+        <f>$P$9*B3*18.02</f>
+        <v>9.8507809402996891</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I24" si="0">1000-H3</f>
+        <v>990.14921905970027</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J24" si="1">E3/I3</f>
+        <v>3.4515057753448405E-3</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K24" si="2">F3/I3</f>
+        <v>3.4515057753448405E-3</v>
+      </c>
+      <c r="L3">
+        <f>((I3-J3*$P$8-K3*$Q$8)/D3)/I3</f>
+        <v>3716.4800627932054</v>
+      </c>
+      <c r="O3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>12</v>
       </c>
@@ -644,18 +734,42 @@
         <v>1.3280000000000001</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D24" si="0">$J$9*(1-B4)</f>
+        <f t="shared" ref="D4:D24" si="3">(C4*$R$8+18.02)*0.000001</f>
+        <v>3.0516016000000002E-4</v>
+      </c>
+      <c r="E4">
+        <f>$P$9*(1-B4)</f>
         <v>2.9850154602394356</v>
       </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E24" si="1">$K$9*(1-B4)</f>
+      <c r="F4">
+        <f>$Q$9*(1-B4)</f>
         <v>2.9850154602394356</v>
       </c>
-      <c r="I4" t="s">
+      <c r="H4">
+        <f>$P$9*B4*18.02</f>
+        <v>17.644255926425117</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>982.3557440735749</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>3.0386298224931727E-3</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="2"/>
+        <v>3.0386298224931727E-3</v>
+      </c>
+      <c r="L4">
+        <f>((I4-J4*$P$8-K4*$Q$8)/D4)/I4</f>
+        <v>3274.4107473318122</v>
+      </c>
+      <c r="O4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>23</v>
       </c>
@@ -666,18 +780,42 @@
         <v>1.581</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>3.5986381999999996E-4</v>
+      </c>
+      <c r="E5">
+        <f>$P$9*(1-B5)</f>
         <v>2.5073337033219696</v>
       </c>
-      <c r="E5">
-        <f t="shared" si="1"/>
+      <c r="F5">
+        <f>$Q$9*(1-B5)</f>
         <v>2.5073337033219696</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="H5">
+        <f>$P$9*B5*18.02</f>
+        <v>26.252081186077856</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>973.74791881392218</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>2.5749310010090066E-3</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>2.5749310010090066E-3</v>
+      </c>
+      <c r="L5">
+        <f>((I5-J5*$P$8-K5*$Q$8)/D5)/I5</f>
+        <v>2776.9752905133882</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>37</v>
       </c>
@@ -688,18 +826,42 @@
         <v>1.9990000000000001</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>4.5024377999999999E-4</v>
+      </c>
+      <c r="E6">
+        <f>$P$9*(1-B6)</f>
         <v>1.9919923888052009</v>
       </c>
-      <c r="E6">
-        <f t="shared" si="1"/>
+      <c r="F6">
+        <f>$Q$9*(1-B6)</f>
         <v>1.9919923888052009</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H6">
+        <f>$P$9*B6*18.02</f>
+        <v>35.538531673670022</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>964.46146832632996</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>2.0653934389540602E-3</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>2.0653934389540602E-3</v>
+      </c>
+      <c r="L6">
+        <f>((I6-J6*$P$8-K6*$Q$8)/D6)/I6</f>
+        <v>2219.8191953213845</v>
+      </c>
+      <c r="O6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>59</v>
       </c>
@@ -710,24 +872,48 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>5.6938099999999999E-4</v>
+      </c>
+      <c r="E7">
+        <f>$P$9*(1-B7)</f>
         <v>1.5539522714659479</v>
       </c>
-      <c r="E7">
-        <f t="shared" si="1"/>
+      <c r="F7">
+        <f>$Q$9*(1-B7)</f>
         <v>1.5539522714659479</v>
       </c>
-      <c r="J7" t="s">
+      <c r="H7">
+        <f>$P$9*B7*18.02</f>
+        <v>43.432014588123359</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>956.56798541187663</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>1.6245079232887467E-3</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>1.6245079232887467E-3</v>
+      </c>
+      <c r="L7">
+        <f>((I7-J7*$P$8-K7*$Q$8)/D7)/I7</f>
+        <v>1755.5408331949529</v>
+      </c>
+      <c r="P7" t="s">
         <v>8</v>
       </c>
-      <c r="K7" t="s">
+      <c r="Q7" t="s">
         <v>9</v>
       </c>
-      <c r="L7" t="s">
+      <c r="R7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>88</v>
       </c>
@@ -738,30 +924,55 @@
         <v>3.19</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>7.0776179999999995E-4</v>
+      </c>
+      <c r="E8">
+        <f>$P$9*(1-B8)</f>
         <v>1.2427654007769762</v>
       </c>
-      <c r="E8">
-        <f t="shared" si="1"/>
+      <c r="F8">
+        <f>$Q$9*(1-B8)</f>
         <v>1.2427654007769762</v>
       </c>
-      <c r="I8" t="s">
+      <c r="H8">
+        <f>$P$9*B8*18.02</f>
+        <v>49.039601997938632</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>950.96039800206131</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>1.3068529492794739E-3</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>1.3068529492794739E-3</v>
+      </c>
+      <c r="L8">
+        <f>((I8-J8*$P$8-K8*$Q$8)/D8)/I8</f>
+        <v>1412.4149295091372</v>
+      </c>
+      <c r="O8" t="s">
         <v>10</v>
       </c>
-      <c r="J8">
+      <c r="P8">
         <v>106.12</v>
       </c>
-      <c r="K8">
+      <c r="Q8">
         <v>146.13999999999999</v>
       </c>
-      <c r="L8" s="2">
-        <v>232.22412</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="R8" s="2">
+        <f>P8+Q8-18.02*2</f>
+        <v>216.22</v>
+      </c>
+      <c r="S8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>129</v>
       </c>
@@ -772,29 +983,53 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>8.8722439999999974E-4</v>
+      </c>
+      <c r="E9">
+        <f>$P$9*(1-B9)</f>
         <v>0.98588757631015633</v>
       </c>
-      <c r="E9">
-        <f t="shared" si="1"/>
+      <c r="F9">
+        <f>$Q$9*(1-B9)</f>
         <v>0.98588757631015633</v>
       </c>
-      <c r="I9" t="s">
+      <c r="H9">
+        <f>$P$9*B9*18.02</f>
+        <v>53.668540394830728</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>946.33145960516924</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>1.0417994311649437E-3</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>1.0417994311649437E-3</v>
+      </c>
+      <c r="L9">
+        <f>((I9-J9*$P$8-K9*$Q$8)/D9)/I9</f>
+        <v>1126.7975626726409</v>
+      </c>
+      <c r="O9" t="s">
         <v>12</v>
       </c>
-      <c r="J9">
-        <f>1000/(J8+K8)</f>
+      <c r="P9">
+        <f>1000/(P8+Q8)</f>
         <v>3.9641639578212957</v>
       </c>
-      <c r="K9">
-        <f>1000/(J8+K8)</f>
+      <c r="Q9">
+        <f>1000/(P8+Q8)</f>
         <v>3.9641639578212957</v>
       </c>
-      <c r="M9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="S9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>170</v>
       </c>
@@ -805,15 +1040,47 @@
         <v>4.75</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>1.045065E-3</v>
+      </c>
+      <c r="E10">
+        <f>$P$9*(1-B10)</f>
         <v>0.83485292951716494</v>
       </c>
-      <c r="E10">
-        <f t="shared" si="1"/>
+      <c r="F10">
+        <f>$Q$9*(1-B10)</f>
         <v>0.83485292951716494</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="H10">
+        <f>$P$9*B10*18.02</f>
+        <v>56.390184730040438</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>943.60981526995954</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>8.8474379558919696E-4</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>8.8474379558919696E-4</v>
+      </c>
+      <c r="L10">
+        <f>((I10-J10*$P$8-K10*$Q$8)/D10)/I10</f>
+        <v>956.65195653068508</v>
+      </c>
+      <c r="P10" s="3">
+        <f>P9*P8</f>
+        <v>420.6770792039959</v>
+      </c>
+      <c r="Q10" s="3">
+        <f>Q9*Q8</f>
+        <v>579.32292079600415</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>203</v>
       </c>
@@ -824,15 +1091,39 @@
         <v>5.44</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>1.1942568000000001E-3</v>
+      </c>
+      <c r="E11">
+        <f>$P$9*(1-B11)</f>
         <v>0.72900975184333605</v>
       </c>
-      <c r="E11">
-        <f t="shared" si="1"/>
+      <c r="F11">
+        <f>$Q$9*(1-B11)</f>
         <v>0.72900975184333605</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="H11">
+        <f>$P$9*B11*18.02</f>
+        <v>58.297478791722831</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>941.70252120827718</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>7.741401721086614E-4</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>7.741401721086614E-4</v>
+      </c>
+      <c r="L11">
+        <f>((I11-J11*$P$8-K11*$Q$8)/D11)/I11</f>
+        <v>837.16720392128536</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>235</v>
       </c>
@@ -843,15 +1134,42 @@
         <v>6.06</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>1.3283131999999999E-3</v>
+      </c>
+      <c r="E12">
+        <f>$P$9*(1-B12)</f>
         <v>0.65448346943629598</v>
       </c>
-      <c r="E12">
-        <f t="shared" si="1"/>
+      <c r="F12">
+        <f>$Q$9*(1-B12)</f>
         <v>0.65448346943629598</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="H12">
+        <f>$P$9*B12*18.02</f>
+        <v>59.640442400697694</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>940.35955759930232</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>6.9599278717086071E-4</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="2"/>
+        <v>6.9599278717086071E-4</v>
+      </c>
+      <c r="L12">
+        <f>((I12-J12*$P$8-K12*$Q$8)/D12)/I12</f>
+        <v>752.69393815229034</v>
+      </c>
+      <c r="O12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>270</v>
       </c>
@@ -862,18 +1180,42 @@
         <v>6.67</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>1.4602074E-3</v>
+      </c>
+      <c r="E13">
+        <f>$P$9*(1-B13)</f>
         <v>0.59462459367319442</v>
       </c>
-      <c r="E13">
-        <f t="shared" si="1"/>
+      <c r="F13">
+        <f>$Q$9*(1-B13)</f>
         <v>0.59462459367319442</v>
       </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="H13">
+        <f>$P$9*B13*18.02</f>
+        <v>60.719099341948777</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>939.28090065805122</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>6.3306364821919209E-4</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>6.3306364821919209E-4</v>
+      </c>
+      <c r="L13">
+        <f>((I13-J13*$P$8-K13*$Q$8)/D13)/I13</f>
+        <v>684.71778727908702</v>
+      </c>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>321</v>
       </c>
@@ -884,15 +1226,39 @@
         <v>7.53</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>1.6461566E-3</v>
+      </c>
+      <c r="E14">
+        <f>$P$9*(1-B14)</f>
         <v>0.52644097359866815</v>
       </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
+      <c r="F14">
+        <f>$Q$9*(1-B14)</f>
         <v>0.52644097359866815</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="H14">
+        <f>$P$9*B14*18.02</f>
+        <v>61.947768175691742</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>938.05223182430825</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>5.61206461366074E-4</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="2"/>
+        <v>5.61206461366074E-4</v>
+      </c>
+      <c r="L14">
+        <f>((I14-J14*$P$8-K14*$Q$8)/D14)/I14</f>
+        <v>607.38393963270312</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>397</v>
       </c>
@@ -903,15 +1269,39 @@
         <v>8.6</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>1.8775119999999998E-3</v>
+      </c>
+      <c r="E15">
+        <f>$P$9*(1-B15)</f>
         <v>0.46103226829461652</v>
       </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
+      <c r="F15">
+        <f>$Q$9*(1-B15)</f>
         <v>0.46103226829461652</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="H15">
+        <f>$P$9*B15*18.02</f>
+        <v>63.126433045270758</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>936.8735669547292</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>4.9209656943698804E-4</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="2"/>
+        <v>4.9209656943698804E-4</v>
+      </c>
+      <c r="L15">
+        <f>((I15-J15*$P$8-K15*$Q$8)/D15)/I15</f>
+        <v>532.5491924584785</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>488</v>
       </c>
@@ -922,15 +1312,39 @@
         <v>9.75</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>2.1261649999999997E-3</v>
+      </c>
+      <c r="E16">
+        <f>$P$9*(1-B16)</f>
         <v>0.40672322207246503</v>
       </c>
-      <c r="E16">
-        <f t="shared" si="1"/>
+      <c r="F16">
+        <f>$Q$9*(1-B16)</f>
         <v>0.40672322207246503</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H16">
+        <f>$P$9*B16*18.02</f>
+        <v>64.105082058193929</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>935.89491794180606</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>4.3458214621671347E-4</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="2"/>
+        <v>4.3458214621671347E-4</v>
+      </c>
+      <c r="L16">
+        <f>((I16-J16*$P$8-K16*$Q$8)/D16)/I16</f>
+        <v>470.27529060379004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>596</v>
       </c>
@@ -941,15 +1355,39 @@
         <v>10.92</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>2.3791424E-3</v>
+      </c>
+      <c r="E17">
+        <f>$P$9*(1-B17)</f>
         <v>0.36311741853643076</v>
       </c>
-      <c r="E17">
-        <f t="shared" si="1"/>
+      <c r="F17">
+        <f>$Q$9*(1-B17)</f>
         <v>0.36311741853643076</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H17">
+        <f>$P$9*B17*18.02</f>
+        <v>64.890858637913269</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>935.10914136208669</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>3.8831554785948442E-4</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="2"/>
+        <v>3.8831554785948442E-4</v>
+      </c>
+      <c r="L17">
+        <f>((I17-J17*$P$8-K17*$Q$8)/D17)/I17</f>
+        <v>420.27549336219982</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>690</v>
       </c>
@@ -960,15 +1398,39 @@
         <v>11.94</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>2.5996867999999998E-3</v>
+      </c>
+      <c r="E18">
+        <f>$P$9*(1-B18)</f>
         <v>0.33180052326964243</v>
       </c>
-      <c r="E18">
-        <f t="shared" si="1"/>
+      <c r="F18">
+        <f>$Q$9*(1-B18)</f>
         <v>0.33180052326964243</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H18">
+        <f>$P$9*B18*18.02</f>
+        <v>65.455189090620792</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>934.54481090937918</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>3.5503971494612089E-4</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="2"/>
+        <v>3.5503971494612089E-4</v>
+      </c>
+      <c r="L18">
+        <f>((I18-J18*$P$8-K18*$Q$8)/D18)/I18</f>
+        <v>384.62485741293716</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>793</v>
       </c>
@@ -979,15 +1441,39 @@
         <v>12.82</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>2.7899603999999999E-3</v>
+      </c>
+      <c r="E19">
+        <f>$P$9*(1-B19)</f>
         <v>0.30920478871006091</v>
       </c>
-      <c r="E19">
-        <f t="shared" si="1"/>
+      <c r="F19">
+        <f>$Q$9*(1-B19)</f>
         <v>0.30920478871006091</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H19">
+        <f>$P$9*B19*18.02</f>
+        <v>65.862364227384447</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>934.13763577261557</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>3.3100560010551426E-4</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="2"/>
+        <v>3.3100560010551426E-4</v>
+      </c>
+      <c r="L19">
+        <f>((I19-J19*$P$8-K19*$Q$8)/D19)/I19</f>
+        <v>358.39598773820722</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>900</v>
       </c>
@@ -998,15 +1484,39 @@
         <v>13.77</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>2.9953694E-3</v>
+      </c>
+      <c r="E20">
+        <f>$P$9*(1-B20)</f>
         <v>0.28819471973360816</v>
       </c>
-      <c r="E20">
-        <f t="shared" si="1"/>
+      <c r="F20">
+        <f>$Q$9*(1-B20)</f>
         <v>0.28819471973360816</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H20">
+        <f>$P$9*B20*18.02</f>
+        <v>66.240965670340131</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>933.75903432965993</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>3.08639283945993E-4</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="2"/>
+        <v>3.08639283945993E-4</v>
+      </c>
+      <c r="L20">
+        <f>((I20-J20*$P$8-K20*$Q$8)/D20)/I20</f>
+        <v>333.82080335260275</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>1008</v>
       </c>
@@ -1017,15 +1527,39 @@
         <v>14.33</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>3.1164525999999998E-3</v>
+      </c>
+      <c r="E21">
+        <f>$P$9*(1-B21)</f>
         <v>0.27630222786014424</v>
       </c>
-      <c r="E21">
-        <f t="shared" si="1"/>
+      <c r="F21">
+        <f>$Q$9*(1-B21)</f>
         <v>0.27630222786014424</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H21">
+        <f>$P$9*B21*18.02</f>
+        <v>66.455268373899941</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>933.54473162610009</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>2.9597106437402918E-4</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="2"/>
+        <v>2.9597106437402918E-4</v>
+      </c>
+      <c r="L21">
+        <f>((I21-J21*$P$8-K21*$Q$8)/D21)/I21</f>
+        <v>320.85199161317991</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>1147</v>
       </c>
@@ -1036,15 +1570,39 @@
         <v>15.478</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>3.3646731599999997E-3</v>
+      </c>
+      <c r="E22">
+        <f>$P$9*(1-B22)</f>
         <v>0.25608499167525567</v>
       </c>
-      <c r="E22">
-        <f t="shared" si="1"/>
+      <c r="F22">
+        <f>$Q$9*(1-B22)</f>
         <v>0.25608499167525567</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H22">
+        <f>$P$9*B22*18.02</f>
+        <v>66.819582969951639</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>933.18041703004837</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>2.7442173774957146E-4</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="2"/>
+        <v>2.7442173774957146E-4</v>
+      </c>
+      <c r="L22">
+        <f>((I22-J22*$P$8-K22*$Q$8)/D22)/I22</f>
+        <v>297.18364012829653</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>1370</v>
       </c>
@@ -1055,15 +1613,39 @@
         <v>16.809999999999999</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>3.6526781999999995E-3</v>
+      </c>
+      <c r="E23">
+        <f>$P$9*(1-B23)</f>
         <v>0.23586775549036709</v>
       </c>
-      <c r="E23">
-        <f t="shared" si="1"/>
+      <c r="F23">
+        <f>$Q$9*(1-B23)</f>
         <v>0.23586775549036709</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H23">
+        <f>$P$9*B23*18.02</f>
+        <v>67.183897566003338</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>932.81610243399666</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>2.5285557879513169E-4</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="2"/>
+        <v>2.5285557879513169E-4</v>
+      </c>
+      <c r="L23">
+        <f>((I23-J23*$P$8-K23*$Q$8)/D23)/I23</f>
+        <v>273.75300147196094</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>1606</v>
       </c>
@@ -1074,18 +1656,42 @@
         <v>18.079999999999998</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
+        <v>3.9272775999999992E-3</v>
+      </c>
+      <c r="E24">
+        <f>$P$9*(1-B24)</f>
         <v>0.21921826686751772</v>
       </c>
-      <c r="E24">
-        <f t="shared" si="1"/>
+      <c r="F24">
+        <f>$Q$9*(1-B24)</f>
         <v>0.21921826686751772</v>
+      </c>
+      <c r="H24">
+        <f>$P$9*B24*18.02</f>
+        <v>67.483921350987075</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>932.51607864901291</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>2.350825598472374E-4</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="2"/>
+        <v>2.350825598472374E-4</v>
+      </c>
+      <c r="L24">
+        <f>((I24-J24*$P$8-K24*$Q$8)/D24)/I24</f>
+        <v>254.61312094088075</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <hyperlinks>
-    <hyperlink ref="I5" r:id="rId1" xr:uid="{D174AFD0-39EB-4DBF-AC0A-971AADEB5EF3}"/>
+    <hyperlink ref="O5" r:id="rId1" xr:uid="{D174AFD0-39EB-4DBF-AC0A-971AADEB5EF3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>